<commit_message>
Upload Territory Data, template
</commit_message>
<xml_diff>
--- a/download/template_upload_leads.xlsx
+++ b/download/template_upload_leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2h\htdocs\CRM-APPS\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1717DB1-6BD1-4DF5-80D8-2DE71167D11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EC13C2-6142-45EA-8D87-548DDE85CCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leadsupload" sheetId="1" r:id="rId1"/>
@@ -298,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -319,6 +319,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -637,14 +639,15 @@
   <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="8" customWidth="1"/>
-    <col min="3" max="5" width="19.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
     <col min="6" max="7" width="19.7109375" style="5" customWidth="1"/>
     <col min="8" max="9" width="19.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
@@ -673,10 +676,10 @@
       <c r="B3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="13" t="s">
         <v>41</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -699,10 +702,10 @@
       <c r="B4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="12">
         <v>123</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="12">
         <v>742</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -725,10 +728,10 @@
       <c r="B5" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="12">
         <v>456</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="12">
         <v>742</v>
       </c>
       <c r="E5" s="10" t="s">

</xml_diff>

<commit_message>
Upload Leads, add generate leads id
</commit_message>
<xml_diff>
--- a/download/template_upload_leads.xlsx
+++ b/download/template_upload_leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2h\htdocs\CRM-APPS\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EC13C2-6142-45EA-8D87-548DDE85CCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650B791E-9D66-4D0C-A8B2-74F538B4C4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leadsupload" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>Platform Data</t>
   </si>
@@ -172,28 +172,25 @@
     <t>E20</t>
   </si>
   <si>
-    <t>Tes Konsumen</t>
-  </si>
-  <si>
-    <t>tes@gmail.com</t>
-  </si>
-  <si>
-    <t>tes2@gmail.com</t>
-  </si>
-  <si>
-    <t>Kota Jambi</t>
-  </si>
-  <si>
-    <t>Gathering / Showroom Event</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>Dealer</t>
-  </si>
-  <si>
-    <t>FINCOY</t>
+    <t>D</t>
+  </si>
+  <si>
+    <t>M. SIGIT LINGGA SAPUTRA</t>
+  </si>
+  <si>
+    <t>m.sigitlingga@gmail.com</t>
+  </si>
+  <si>
+    <t>MUHAMMAD HARITS</t>
+  </si>
+  <si>
+    <t>HARITS@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>081228715882</t>
+  </si>
+  <si>
+    <t>081366328464</t>
   </si>
 </sst>
 </file>
@@ -298,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -321,6 +318,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -636,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H69"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,7 +645,7 @@
     <col min="1" max="1" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" style="8" customWidth="1"/>
     <col min="3" max="4" width="19.7109375" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="19.7109375" style="5" customWidth="1"/>
     <col min="8" max="9" width="19.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
@@ -666,7 +664,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="8">
-        <v>20</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -699,61 +697,57 @@
       <c r="A4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1571</v>
+      </c>
+      <c r="G4" s="11">
+        <v>2</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="12">
-        <v>123</v>
-      </c>
-      <c r="D4" s="12">
-        <v>742</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="C5" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="F5" s="1">
+        <v>1571</v>
+      </c>
+      <c r="G5" s="11">
+        <v>2</v>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="12">
-        <v>456</v>
-      </c>
-      <c r="D5" s="12">
-        <v>742</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="13.35" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E8" s="2"/>
@@ -786,9 +780,9 @@
       <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -798,9 +792,9 @@
       <c r="H14" s="3"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1026,12 +1020,12 @@
       <c r="H52" s="3"/>
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="2"/>
       <c r="H53" s="3"/>
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
       <c r="H54" s="3"/>
     </row>
     <row r="55" spans="5:8" x14ac:dyDescent="0.25">
@@ -1117,12 +1111,6 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
       <c r="H68" s="3"/>
-    </row>
-    <row r="69" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="2"/>
-      <c r="H69" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:H3" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
@@ -1133,7 +1121,7 @@
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E4" r:id="rId1" xr:uid="{3369A5C0-22ED-4FDB-9B92-D813FF3458BB}"/>
-    <hyperlink ref="E5" r:id="rId2" xr:uid="{3957F3E3-2F72-4405-AA0B-4620B7385B64}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{D4D592EA-6D8F-4162-84AF-BB100ABDFB1F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Lead, fix bugs validation
</commit_message>
<xml_diff>
--- a/download/template_upload_leads.xlsx
+++ b/download/template_upload_leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2h\htdocs\CRM-APPS\download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650B791E-9D66-4D0C-A8B2-74F538B4C4C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAC2EA4-C5E8-45A6-B876-90C5A5904DC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="leadsupload" sheetId="1" r:id="rId1"/>
@@ -637,7 +637,7 @@
   <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A6" sqref="A6:XFD156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>